<commit_message>
updates analysis of open-ended questions
</commit_message>
<xml_diff>
--- a/userstudy_data_and_analysis/analysis_open_ended/Analysis_open_ended.xlsx
+++ b/userstudy_data_and_analysis/analysis_open_ended/Analysis_open_ended.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/evdoxia_taka_glasgow_ac_uk/Documents/MyDocuments/WAMLS/Deb-Evdoxia-Tanaya/userStudy/Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evdoxiataka\codes\waml_user_study1_analysis\analysis_open_ended\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{E02F7390-64AF-427D-82E4-C022C3FE0DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB611F2A-8674-47D4-8668-EEE22E911EAA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6340AB46-A6B2-409B-BBB4-70943937DFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -282,7 +282,225 @@
 It's also unclear how 'on screen appearances' are defined--like if a character leaves the scene and then comes back does that count as two? Is it collating information from extras visible in crowd or public scenes? Does that data even matter to most viewers?  </t>
   </si>
   <si>
-    <t>I don't know what films these are based on for me to double-check - that's why I'm not very confident in the AI's judgement (looking at the bottom charts - the AI is very close to the ground truth so that increases my confidence now). 
+    <t>I think the description of male or females over 50 should’ve been specified. 
+I liked the figures below the pie chart</t>
+  </si>
+  <si>
+    <t>I think the interface is confusing. 
+The way that the two pie charts (for age and gender) were combined was difficult for me to read and understand.</t>
+  </si>
+  <si>
+    <t>i guess the way in which the pie chart was presented made it a bit confusing with having both pieces of information in one chart but it is efficient. 
+the hover features definitely made it a lot easier to interpret so that was helpful. 
+i didnt fully understand the how i would be able to use the data of bias given but i do know it serves purpose.</t>
+  </si>
+  <si>
+    <t>It seems to predict gender and age accurately to an extent, 
+however a better represenation instead of pie charts could be used to avoid confusion</t>
+  </si>
+  <si>
+    <t>Presentation needs improvement</t>
+  </si>
+  <si>
+    <t>Not categorized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disliked- 1) I did not find the pie chars to be interactive. They were visually great but there was nothing interactive about them.   
+2) I found the questions to be a bit difficult to answer. For Q2 and Q3, even after reading them 4 times, I was confused about what was asked.  
+3) There was no information on male appearances in the pie charts yet males were an option to a question's answer  
+4) There was no mention of who was Over 50's- Males or females?   
+Liked-  Information was presented in a very neat and clean manner.  
+There had to be some thinking before answering the question so there was slight cognitive load. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think I would find it more interesting in context, and would like to see what the films are. 
+I wasn't completely sure what was being represented, if it was related to the different characters or just any appearance of a face. </t>
+  </si>
+  <si>
+    <t>I would like to know the films
+Percentages calculation confusion</t>
+  </si>
+  <si>
+    <t>I think it is a cool tool, 
+and it's impressive how accurate it seems to be, at least when looking at the aggregate information</t>
+  </si>
+  <si>
+    <t>Not really. 
+I overall like this tool.</t>
+  </si>
+  <si>
+    <t>Doughnut charts not appropriate
+Suggestion for improvement
+Presentation is confusing/hard-to-read or understand - nesting rings</t>
+  </si>
+  <si>
+    <t>Presentation is confusing/hard-to-read or understand, Suggestion for improvement</t>
+  </si>
+  <si>
+    <t>Presentation is confusing/hard-to-read or understand - too much information
+Not categorized
+Hover - not liking it
+Percentages calculation confusion</t>
+  </si>
+  <si>
+    <t>Presentation is confusing/hard-to-read or understand
+Presentation is confusing/hard-to-read or understand - nesting rings</t>
+  </si>
+  <si>
+    <t>Confusing bias/confidence with accuracy
+Presentation is confusing/hard-to-read or understand - Doughnut charts not appropriate, Presentation needs improvement</t>
+  </si>
+  <si>
+    <t>Presentation is confusing/hard-to-read or understand - color coding</t>
+  </si>
+  <si>
+    <t>Presentation is confusing/hard-to-read or understand, Presentation needs improvement</t>
+  </si>
+  <si>
+    <t>I am not sure if it would be very useful to me, without knowing who the actors are. 
+Personally, I watch movies based on the cast quality, not distribution based on gender or age. 
+It can be more useful along side the regular information like cast, just for information purposes I suppose.</t>
+  </si>
+  <si>
+    <t>research</t>
+  </si>
+  <si>
+    <t>Wouldn't use it</t>
+  </si>
+  <si>
+    <t>Little idea about the applicability</t>
+  </si>
+  <si>
+    <t>I wouldn't use it. 
+Representation is very important, but I'm not convinced that the best way to get there is through numerical comparisons. 
+I also don't think AI in general is worth the massive amount of resources it drains.</t>
+  </si>
+  <si>
+    <t>research, within a films context</t>
+  </si>
+  <si>
+    <t>within a films context</t>
+  </si>
+  <si>
+    <t>outside a films context</t>
+  </si>
+  <si>
+    <t>within a films context, research</t>
+  </si>
+  <si>
+    <t>I don't check for movie analytics so I can't think of a use case. 
+I'd just want it to be able to quick to answer my written queries directly but  offer an option for me to check the whole visualisation if I wanted to reassure myself a bit more.</t>
+  </si>
+  <si>
+    <t>not sure if I would use it
+not interested in this info - I like to know about the cast primarily
+within a films context</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I wouldn't use it because I don't know that this sort of information is important beyond the main cast of any given film. 
+There are so many ways this data could be skewed and just having data on gender and age doesn't mean a film reflects positively on the demographics represented. For example, movies like Seven Brides for Seven Brothers would have high instances of women on screen, but that doesn't mean the depicitons of women are positive, so to me, a tool like this has absolutely no practical use without further detail provided. Or like in horror movies--yes, there may be many women on screen, but are they all there because they're being tortured and murdered? A tool like this ignores the context in which people appear on screen and would end up generating a lot of false positives in terms of contemporary metrics of representation--it's not enough to just count how many women appear on screen anymore. We need to consider *how* they're depicted. </t>
+  </si>
+  <si>
+    <t>Wouldn't use it, not interested in this info - I like to know about the cast primarily
+Counts of representation cannot account for how characters are represented</t>
+  </si>
+  <si>
+    <t>not interested in this information
+within a films context</t>
+  </si>
+  <si>
+    <t>Wouldn't use it, not interested in this information</t>
+  </si>
+  <si>
+    <t>Wouldn't use it
+Counts of representation cannot account for how characters are represented
+AI skepticism</t>
+  </si>
+  <si>
+    <t>Positive comment
+Not categorized</t>
+  </si>
+  <si>
+    <t>Positive comment - tool
+Understanding needs time
+Info icons - simpler and more descriptive</t>
+  </si>
+  <si>
+    <t>Positive comment</t>
+  </si>
+  <si>
+    <t>Misunderstanding/lack of understanding of UI elements
+Not categorized
+Misunderstanding/lack of understanding of UI elements
+Misunderstanding/lack of understanding of UI elements
+Positive comment - presentation
+Not categorized</t>
+  </si>
+  <si>
+    <t>Positive comment - tool
+Confusing bias/confidence with accuracy</t>
+  </si>
+  <si>
+    <t>Positive comment - presentation</t>
+  </si>
+  <si>
+    <t>Positive comment - tool</t>
+  </si>
+  <si>
+    <t>Not categorized
+Positive comment - tool</t>
+  </si>
+  <si>
+    <t>For a movie that I am intending to watch I would rather read reviews about how the chracteres are presented and portrayed. Quantiative measures feel meaningless to me in this circumnstances, the numbers do not mean any specific thing. I am intrested in what a movie presents and with what qualitites rather than any measurments.</t>
+  </si>
+  <si>
+    <t>I would not</t>
+  </si>
+  <si>
+    <t>Counts of representation cannot account for how characters are represented</t>
+  </si>
+  <si>
+    <t>Analyse temporal trends over the decades - in films from different countries, cultures, languages, regions - 
+Develop it further to recognise race, language etc. 
+Study shifts in representation over time. 
+Expand it to identify shades of characters (e.g. hero/villain, positive/negative roles, victim/perpretator etc.). 
+I could probably come up with many others if I think longer about it.</t>
+  </si>
+  <si>
+    <t>within a films context
+More demographics
+Counts of representation cannot account for how characters are represented
+Counts of representation cannot account for how characters are represented
+Not categorized</t>
+  </si>
+  <si>
+    <t>More demographics</t>
+  </si>
+  <si>
+    <t>Understanding needs time
+Color coding, Positive comment - presentation
+Info icons - useful, Positive comment</t>
+  </si>
+  <si>
+    <t>Positive comment - tool
+Overload by the number of films shown
+Presentation is confusing/hard-to-read or understand - color coding, Suggestion for improvement
+Hover - not useful, Suggestion for improvement
+Bias presentation - usefulness, Positive comment
+More demographics</t>
+  </si>
+  <si>
+    <t>Presentation is confusing/hard-to-read or understand - nesting rings
+Hover - useful, Positive comment
+Bias presentation - could not understand how to use this info</t>
+  </si>
+  <si>
+    <t>Misunderstanding/lack of understanding of UI elements
+Bias presentation - liking, Positive comment</t>
+  </si>
+  <si>
+    <t>I don't know what films these are based on for me to double-check - that's why I'm not very confident in the AI's judgement 
+(looking at the bottom charts - the AI is very close to the ground truth so that increases my confidence now). 
 UI can make it easier to understand - 
 for example, using icons to represent gender and age reduces cognitive load; 
 similarly, displaying three graphs in the same row can feel mentally taxing to read and can be eased by giving control to cycle through them or similar. 
@@ -294,207 +512,8 @@
 One thing I might be interested to see added is extra demographics like ethnicity.</t>
   </si>
   <si>
-    <t>I think the description of male or females over 50 should’ve been specified. 
-I liked the figures below the pie chart</t>
-  </si>
-  <si>
-    <t>I think the interface is confusing. 
-The way that the two pie charts (for age and gender) were combined was difficult for me to read and understand.</t>
-  </si>
-  <si>
-    <t>i guess the way in which the pie chart was presented made it a bit confusing with having both pieces of information in one chart but it is efficient. 
-the hover features definitely made it a lot easier to interpret so that was helpful. 
-i didnt fully understand the how i would be able to use the data of bias given but i do know it serves purpose.</t>
-  </si>
-  <si>
-    <t>It seems to predict gender and age accurately to an extent, 
-however a better represenation instead of pie charts could be used to avoid confusion</t>
-  </si>
-  <si>
-    <t>Presentation needs improvement</t>
-  </si>
-  <si>
-    <t>Not categorized</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Disliked- 1) I did not find the pie chars to be interactive. They were visually great but there was nothing interactive about them.   
-2) I found the questions to be a bit difficult to answer. For Q2 and Q3, even after reading them 4 times, I was confused about what was asked.  
-3) There was no information on male appearances in the pie charts yet males were an option to a question's answer  
-4) There was no mention of who was Over 50's- Males or females?   
-Liked-  Information was presented in a very neat and clean manner.  
-There had to be some thinking before answering the question so there was slight cognitive load. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I think I would find it more interesting in context, and would like to see what the films are. 
-I wasn't completely sure what was being represented, if it was related to the different characters or just any appearance of a face. </t>
-  </si>
-  <si>
     <t>I would like to know the films
-Percentages calculation confusion</t>
-  </si>
-  <si>
-    <t>I think it is a cool tool, 
-and it's impressive how accurate it seems to be, at least when looking at the aggregate information</t>
-  </si>
-  <si>
-    <t>Not really. 
-I overall like this tool.</t>
-  </si>
-  <si>
-    <t>Doughnut charts not appropriate
-Suggestion for improvement
-Presentation is confusing/hard-to-read or understand - nesting rings</t>
-  </si>
-  <si>
-    <t>Presentation is confusing/hard-to-read or understand, Suggestion for improvement</t>
-  </si>
-  <si>
-    <t>Presentation is confusing/hard-to-read or understand - too much information
-Not categorized
-Hover - not liking it
-Percentages calculation confusion</t>
-  </si>
-  <si>
-    <t>Presentation is confusing/hard-to-read or understand
-Presentation is confusing/hard-to-read or understand - nesting rings</t>
-  </si>
-  <si>
-    <t>Confusing bias/confidence with accuracy
-Presentation is confusing/hard-to-read or understand - Doughnut charts not appropriate, Presentation needs improvement</t>
-  </si>
-  <si>
-    <t>Presentation is confusing/hard-to-read or understand - color coding</t>
-  </si>
-  <si>
-    <t>Presentation is confusing/hard-to-read or understand, Presentation needs improvement</t>
-  </si>
-  <si>
-    <t>I am not sure if it would be very useful to me, without knowing who the actors are. 
-Personally, I watch movies based on the cast quality, not distribution based on gender or age. 
-It can be more useful along side the regular information like cast, just for information purposes I suppose.</t>
-  </si>
-  <si>
-    <t>research</t>
-  </si>
-  <si>
-    <t>Wouldn't use it</t>
-  </si>
-  <si>
-    <t>Little idea about the applicability</t>
-  </si>
-  <si>
-    <t>I wouldn't use it. 
-Representation is very important, but I'm not convinced that the best way to get there is through numerical comparisons. 
-I also don't think AI in general is worth the massive amount of resources it drains.</t>
-  </si>
-  <si>
-    <t>research, within a films context</t>
-  </si>
-  <si>
-    <t>within a films context</t>
-  </si>
-  <si>
-    <t>outside a films context</t>
-  </si>
-  <si>
-    <t>within a films context, research</t>
-  </si>
-  <si>
-    <t>I don't check for movie analytics so I can't think of a use case. 
-I'd just want it to be able to quick to answer my written queries directly but  offer an option for me to check the whole visualisation if I wanted to reassure myself a bit more.</t>
-  </si>
-  <si>
-    <t>not sure if I would use it
-not interested in this info - I like to know about the cast primarily
-within a films context</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I wouldn't use it because I don't know that this sort of information is important beyond the main cast of any given film. 
-There are so many ways this data could be skewed and just having data on gender and age doesn't mean a film reflects positively on the demographics represented. For example, movies like Seven Brides for Seven Brothers would have high instances of women on screen, but that doesn't mean the depicitons of women are positive, so to me, a tool like this has absolutely no practical use without further detail provided. Or like in horror movies--yes, there may be many women on screen, but are they all there because they're being tortured and murdered? A tool like this ignores the context in which people appear on screen and would end up generating a lot of false positives in terms of contemporary metrics of representation--it's not enough to just count how many women appear on screen anymore. We need to consider *how* they're depicted. </t>
-  </si>
-  <si>
-    <t>Wouldn't use it, not interested in this info - I like to know about the cast primarily
-Counts of representation cannot account for how characters are represented</t>
-  </si>
-  <si>
-    <t>not interested in this information
-within a films context</t>
-  </si>
-  <si>
-    <t>Wouldn't use it, not interested in this information</t>
-  </si>
-  <si>
-    <t>Wouldn't use it
-Counts of representation cannot account for how characters are represented
-AI skepticism</t>
-  </si>
-  <si>
-    <t>Positive comment
-Not categorized</t>
-  </si>
-  <si>
-    <t>Positive comment - tool
-Understanding needs time
-Info icons - simpler and more descriptive</t>
-  </si>
-  <si>
-    <t>Positive comment</t>
-  </si>
-  <si>
-    <t>Misunderstanding/lack of understanding of UI elements
-Not categorized
-Misunderstanding/lack of understanding of UI elements
-Misunderstanding/lack of understanding of UI elements
-Positive comment - presentation
-Not categorized</t>
-  </si>
-  <si>
-    <t>Positive comment - tool
-Confusing bias/confidence with accuracy</t>
-  </si>
-  <si>
-    <t>Positive comment - presentation</t>
-  </si>
-  <si>
-    <t>Positive comment - tool</t>
-  </si>
-  <si>
-    <t>Not categorized
-Positive comment - tool</t>
-  </si>
-  <si>
-    <t>For a movie that I am intending to watch I would rather read reviews about how the chracteres are presented and portrayed. Quantiative measures feel meaningless to me in this circumnstances, the numbers do not mean any specific thing. I am intrested in what a movie presents and with what qualitites rather than any measurments.</t>
-  </si>
-  <si>
-    <t>I would not</t>
-  </si>
-  <si>
-    <t>Counts of representation cannot account for how characters are represented</t>
-  </si>
-  <si>
-    <t>Analyse temporal trends over the decades - in films from different countries, cultures, languages, regions - 
-Develop it further to recognise race, language etc. 
-Study shifts in representation over time. 
-Expand it to identify shades of characters (e.g. hero/villain, positive/negative roles, victim/perpretator etc.). 
-I could probably come up with many others if I think longer about it.</t>
-  </si>
-  <si>
-    <t>within a films context
-More demographics
-Counts of representation cannot account for how characters are represented
-Counts of representation cannot account for how characters are represented
-Not categorized</t>
-  </si>
-  <si>
-    <t>More demographics</t>
-  </si>
-  <si>
-    <t>Understanding needs time
-Color coding, Positive comment - presentation
-Info icons - useful, Positive comment</t>
-  </si>
-  <si>
-    <t>I would like to know the films
+Bias presentation - usefulness
 Presentation needs improvement
 Suggestion for improvement
 Overload by the number of films shown
@@ -504,23 +523,6 @@
 Suggestion for improvement
 Info icons - liking, Suggestion for improvement, Positive comment
 More demographics</t>
-  </si>
-  <si>
-    <t>Positive comment - tool
-Overload by the number of films shown
-Presentation is confusing/hard-to-read or understand - color coding, Suggestion for improvement
-Hover - not useful, Suggestion for improvement
-Bias presentation - usefulness, Positive comment
-More demographics</t>
-  </si>
-  <si>
-    <t>Presentation is confusing/hard-to-read or understand - nesting rings
-Hover - useful, Positive comment
-Bias presentation - could not understand how to use this info</t>
-  </si>
-  <si>
-    <t>Misunderstanding/lack of understanding of UI elements
-Bias presentation - liking, Positive comment</t>
   </si>
 </sst>
 </file>
@@ -922,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,13 +968,13 @@
         <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -986,13 +988,13 @@
         <v>74</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="180" x14ac:dyDescent="0.25">
@@ -1006,13 +1008,13 @@
         <v>75</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1026,13 +1028,13 @@
         <v>76</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1046,13 +1048,13 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.25">
@@ -1066,13 +1068,13 @@
         <v>77</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1086,13 +1088,13 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1112,7 +1114,7 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="153" customHeight="1" x14ac:dyDescent="0.25">
@@ -1126,13 +1128,13 @@
         <v>79</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="374.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1143,16 +1145,16 @@
         <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>80</v>
+        <v>132</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1163,16 +1165,16 @@
         <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1183,16 +1185,16 @@
         <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1203,16 +1205,16 @@
         <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1223,16 +1225,16 @@
         <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1246,13 +1248,13 @@
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1266,13 +1268,13 @@
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>35</v>
       </c>
       <c r="F17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1286,13 +1288,13 @@
         <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1306,13 +1308,13 @@
         <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="165" x14ac:dyDescent="0.25">
@@ -1323,10 +1325,10 @@
         <v>42</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>43</v>
@@ -1340,16 +1342,16 @@
         <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1363,13 +1365,13 @@
         <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>48</v>
       </c>
       <c r="F22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1380,16 +1382,16 @@
         <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1403,13 +1405,13 @@
         <v>52</v>
       </c>
       <c r="D24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1423,13 +1425,13 @@
         <v>55</v>
       </c>
       <c r="D25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1443,13 +1445,13 @@
         <v>58</v>
       </c>
       <c r="D26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>59</v>
       </c>
       <c r="F26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1463,13 +1465,13 @@
         <v>61</v>
       </c>
       <c r="D27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>62</v>
       </c>
       <c r="F27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1483,13 +1485,13 @@
         <v>64</v>
       </c>
       <c r="D28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1503,13 +1505,13 @@
         <v>67</v>
       </c>
       <c r="D29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1520,16 +1522,16 @@
         <v>69</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>70</v>
       </c>
       <c r="F30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1540,16 +1542,16 @@
         <v>59</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D31" t="s">
-        <v>125</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="F31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>